<commit_message>
Atualização da checklist 10 aspectos: modal versão ingles
</commit_message>
<xml_diff>
--- a/checklists/en/10_functional_aspects.xlsx
+++ b/checklists/en/10_functional_aspects.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgefernandes/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victoriasantos/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00116229-D868-4041-9C6F-BCE723DDA4CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="LB4TBYcSkZl4o5QZAc0KHgbcEIijbDOhUeZor5rsraC8wKbuE007QmHmwvsLkfYR0M2ocdkiesI8FjeSrsPjFw==" workbookSaltValue="7U6EahoqJjuGOnemAfPI4w==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B5F476-54A2-FD46-9591-7BFBA0C1E30C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="3PNpdSFuSRaCmOGa2qpP/0r1n4HwduYIO5kg/n6GRV9gKster4MQXsgtAtdm2YobsVou9GVIu1FuMiwE3PvSyA==" workbookSaltValue="zCeXk19IJZkjwZnS3JibMA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20980" windowHeight="19520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="23500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,10 @@
     <sheet name="8.4" sheetId="29" r:id="rId22"/>
     <sheet name="8.5" sheetId="25" r:id="rId23"/>
     <sheet name="9.1" sheetId="26" r:id="rId24"/>
-    <sheet name="10.1" sheetId="27" r:id="rId25"/>
+    <sheet name="9.2" sheetId="31" r:id="rId25"/>
+    <sheet name="9.3" sheetId="32" r:id="rId26"/>
+    <sheet name="9.4" sheetId="33" r:id="rId27"/>
+    <sheet name="10.1" sheetId="27" r:id="rId28"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -67,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="105">
   <si>
     <t>10 functional aspects Checklist</t>
   </si>
@@ -193,12 +196,6 @@
   </si>
   <si>
     <t xml:space="preserve">8.5 The page layout is done without using the element &lt;table&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">9 - HTML SYNTAX </t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.1 The page must not contain any (x)HTML syntax errors. </t>
   </si>
   <si>
     <t>10 - PDF FILES</t>
@@ -345,12 +342,6 @@
     <t>A estrutura de composição gráfica da página não é feita recorrendo a elementos de tabela mas sim a uma maior diversidade de elementos semânticos (por ex., &lt;main&gt;) e genéricos (por ex., &lt;div&gt;), que permitem a recomposição visual para diferentes tipos e dimensões de ecrã.</t>
   </si>
   <si>
-    <t xml:space="preserve">9 - HTML SYNTAX 						</t>
-  </si>
-  <si>
-    <t>A página não deve apresentar erros de sintaxe de (x)HTML.</t>
-  </si>
-  <si>
     <t xml:space="preserve">10 - PDF FILES								</t>
   </si>
   <si>
@@ -373,6 +364,36 @@
   </si>
   <si>
     <t>YOU CAN EVEN REMOVE THE YELLOW BACKGROUND.</t>
+  </si>
+  <si>
+    <t>9 - MODAL DIALOG</t>
+  </si>
+  <si>
+    <t>9.1 When a modal dialog is open, the focus order goes to an element of the modal</t>
+  </si>
+  <si>
+    <t>9.2 When a modal dialog is open, the keyboard focus  (browser or assistive technologies) must be contained within the elements of the modal</t>
+  </si>
+  <si>
+    <t>9.3 The modal dialog must have a mechanism to close it using a keyboard or any pointing device</t>
+  </si>
+  <si>
+    <t>9.4 When a modal dialog is closed, the focus must return to the interactive element that invoked the modal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 - MODAL DIALOG		</t>
+  </si>
+  <si>
+    <t>If the modal overlaps the browser window, the browser focus must be moved to an element that is contained within the modal.</t>
+  </si>
+  <si>
+    <t>When a modal dialog is open, all elements outside the modal must be inactive. Interactive elements, such as links, buttons or editing fields that appear outside the modal, must not be focused with the mouse or keyboard as well. If a screen reader announced content outside the modal, it means something is wrong.</t>
+  </si>
+  <si>
+    <t>The modal must have a way for the user to close it. This could be a button labeled “Close” and the keyboard shortcut “ESC”.</t>
+  </si>
+  <si>
+    <t>When the modal is closed, it's useful for the user to return to the element that invoked it. A modal is an intermediate window that overlays the primary window. After interaction with the modal, the user must return to the same point from which they left.</t>
   </si>
 </sst>
 </file>
@@ -2041,6 +2062,204 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>126999</xdr:colOff>
       <xdr:row>7</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>707790</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1" descr="ontacte a equipa da Unidade ACESSO da AMA">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD775700-E2E6-E34F-BA32-538D7DC93728}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1130299" y="1752600"/>
+          <a:ext cx="3298591" cy="2184400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing25.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>126999</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>707790</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1" descr="ontacte a equipa da Unidade ACESSO da AMA">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A03CC833-B667-1F41-9B67-8BBC62AD0D9A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1130299" y="1752600"/>
+          <a:ext cx="3273191" cy="2184400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing26.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>126999</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>707790</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1" descr="ontacte a equipa da Unidade ACESSO da AMA">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A93B8BF0-1020-1847-8A61-85E36C978F87}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1130299" y="1752600"/>
+          <a:ext cx="3298591" cy="2184400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing27.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>126999</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
@@ -2825,10 +3044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:Q80"/>
+  <dimension ref="B1:Q83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:O5"/>
+      <selection activeCell="F45" sqref="F45:Q45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2977,11 +3196,11 @@
     <row r="12" spans="2:17" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="13" t="str">
         <f>IF('1.1'!$B$3="x","x"," ")</f>
-        <v xml:space="preserve"> </v>
+        <v>x</v>
       </c>
       <c r="C12" s="13" t="str">
         <f>IF('1.1'!$C$3="x","x"," ")</f>
-        <v>x</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D12" s="13" t="str">
         <f>IF('1.1'!$D$3="x", "x", " ")</f>
@@ -3727,7 +3946,7 @@
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
       <c r="E41" s="29" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="F41" s="30"/>
       <c r="G41" s="30"/>
@@ -3756,7 +3975,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="F42" s="27" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="G42" s="27"/>
       <c r="H42" s="27"/>
@@ -3771,113 +3990,176 @@
       <c r="Q42" s="27"/>
     </row>
     <row r="43" spans="2:17" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="11"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="F43" s="30"/>
-      <c r="G43" s="30"/>
-      <c r="H43" s="30"/>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
-      <c r="K43" s="30"/>
-      <c r="L43" s="30"/>
-      <c r="M43" s="30"/>
-      <c r="N43" s="30"/>
-      <c r="O43" s="30"/>
-      <c r="P43" s="30"/>
-      <c r="Q43" s="31"/>
+      <c r="B43" s="13" t="str">
+        <f>IF('9.2'!$B$3="x","x"," ")</f>
+        <v>x</v>
+      </c>
+      <c r="C43" s="13" t="str">
+        <f>IF('9.2'!$C$3="x","x"," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D43" s="13" t="str">
+        <f>IF('9.2'!$D$3="x", "x", " ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F43" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="27"/>
+      <c r="M43" s="27"/>
+      <c r="N43" s="27"/>
+      <c r="O43" s="27"/>
+      <c r="P43" s="27"/>
+      <c r="Q43" s="27"/>
     </row>
     <row r="44" spans="2:17" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="13" t="str">
+        <f>IF('9.3'!$B$3="x","x"," ")</f>
+        <v>x</v>
+      </c>
+      <c r="C44" s="13" t="str">
+        <f>IF('9.3'!$C$3="x","x"," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D44" s="13" t="str">
+        <f>IF('9.3'!$D$3="x", "x", " ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F44" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="27"/>
+      <c r="L44" s="27"/>
+      <c r="M44" s="27"/>
+      <c r="N44" s="27"/>
+      <c r="O44" s="27"/>
+      <c r="P44" s="27"/>
+      <c r="Q44" s="27"/>
+    </row>
+    <row r="45" spans="2:17" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="13" t="str">
+        <f>IF('9.4'!$B$3="x","x"," ")</f>
+        <v>x</v>
+      </c>
+      <c r="C45" s="13" t="str">
+        <f>IF('9.4'!$C$3="x","x"," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D45" s="13" t="str">
+        <f>IF('9.4'!$D$3="x", "x", " ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F45" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="G45" s="27"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
+      <c r="K45" s="27"/>
+      <c r="L45" s="27"/>
+      <c r="M45" s="27"/>
+      <c r="N45" s="27"/>
+      <c r="O45" s="27"/>
+      <c r="P45" s="27"/>
+      <c r="Q45" s="27"/>
+    </row>
+    <row r="46" spans="2:17" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="11"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="F46" s="30"/>
+      <c r="G46" s="30"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
+      <c r="K46" s="30"/>
+      <c r="L46" s="30"/>
+      <c r="M46" s="30"/>
+      <c r="N46" s="30"/>
+      <c r="O46" s="30"/>
+      <c r="P46" s="30"/>
+      <c r="Q46" s="31"/>
+    </row>
+    <row r="47" spans="2:17" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="13" t="str">
         <f>IF('10.1'!$B$3="x","x"," ")</f>
         <v>x</v>
       </c>
-      <c r="C44" s="13" t="str">
+      <c r="C47" s="13" t="str">
         <f>IF('10.1'!$C$3="x","x"," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D44" s="13" t="str">
+      <c r="D47" s="13" t="str">
         <f>IF('10.1'!$D$3="x", "x", " ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F44" s="28" t="s">
+      <c r="F47" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="G47" s="28"/>
+      <c r="H47" s="28"/>
+      <c r="I47" s="28"/>
+      <c r="J47" s="28"/>
+      <c r="K47" s="28"/>
+      <c r="L47" s="28"/>
+      <c r="M47" s="28"/>
+      <c r="N47" s="28"/>
+      <c r="O47" s="28"/>
+      <c r="P47" s="28"/>
+      <c r="Q47" s="28"/>
+    </row>
+    <row r="51" spans="6:11" ht="34" x14ac:dyDescent="0.4">
+      <c r="F51" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F52" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G44" s="28"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="28"/>
-      <c r="J44" s="28"/>
-      <c r="K44" s="28"/>
-      <c r="L44" s="28"/>
-      <c r="M44" s="28"/>
-      <c r="N44" s="28"/>
-      <c r="O44" s="28"/>
-      <c r="P44" s="28"/>
-      <c r="Q44" s="28"/>
-    </row>
-    <row r="48" spans="2:17" ht="34" x14ac:dyDescent="0.4">
-      <c r="F48" s="2" t="s">
+      <c r="G52" s="26"/>
+      <c r="H52">
+        <f>COUNTIF(D12:D47,"x")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F53" s="26" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F49" s="26" t="s">
+      <c r="G53" s="26"/>
+      <c r="H53">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54" spans="6:11" ht="31" x14ac:dyDescent="0.35">
+      <c r="H54" s="3">
+        <f>COUNTIF($B$12:$B$47,"x")/(H53-COUNTIF($D$12:$D$47,"x"))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F56" t="s">
         <v>47</v>
       </c>
-      <c r="G49" s="26"/>
-      <c r="H49">
-        <f>COUNTIF(D12:D44,"x")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F50" s="26" t="s">
+    </row>
+    <row r="58" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="G58" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="G50" s="26"/>
-      <c r="H50">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="51" spans="6:11" ht="31" x14ac:dyDescent="0.35">
-      <c r="H51" s="3">
-        <f>COUNTIF($B$12:$B$44,"x")/(H50-COUNTIF($D$12:$D$44,"x"))</f>
-        <v>0.95833333333333337</v>
-      </c>
-    </row>
-    <row r="53" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F53" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="55" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="G55" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="H55" s="36"/>
-      <c r="I55" s="36"/>
-      <c r="J55" s="36"/>
-      <c r="K55" s="36"/>
-    </row>
-    <row r="56" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="G56" s="36"/>
-      <c r="H56" s="36"/>
-      <c r="I56" s="36"/>
-      <c r="J56" s="36"/>
-      <c r="K56" s="36"/>
-    </row>
-    <row r="57" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="G57" s="36"/>
-      <c r="H57" s="36"/>
-      <c r="I57" s="36"/>
-      <c r="J57" s="36"/>
-      <c r="K57" s="36"/>
-    </row>
-    <row r="58" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="G58" s="36"/>
       <c r="H58" s="36"/>
       <c r="I58" s="36"/>
       <c r="J58" s="36"/>
@@ -4037,14 +4319,35 @@
       <c r="J80" s="36"/>
       <c r="K80" s="36"/>
     </row>
+    <row r="81" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G81" s="36"/>
+      <c r="H81" s="36"/>
+      <c r="I81" s="36"/>
+      <c r="J81" s="36"/>
+      <c r="K81" s="36"/>
+    </row>
+    <row r="82" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G82" s="36"/>
+      <c r="H82" s="36"/>
+      <c r="I82" s="36"/>
+      <c r="J82" s="36"/>
+      <c r="K82" s="36"/>
+    </row>
+    <row r="83" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G83" s="36"/>
+      <c r="H83" s="36"/>
+      <c r="I83" s="36"/>
+      <c r="J83" s="36"/>
+      <c r="K83" s="36"/>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="FwiZ4MNZ1o5paaawf95b6ugmxK1y+QwJJ4xU0Vc3XJcUE2Z5eDOqq4iw3UTy+GmEkJBwDaQqUCeN78CB4shMpw==" saltValue="Tf5HnigjQ3P/3BEZOgpV6Q==" spinCount="100000" sheet="1" selectLockedCells="1"/>
-  <mergeCells count="45">
-    <mergeCell ref="G55:K80"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="KEoeSQ+074NrMC4tmlV5lW0iMFa0nnxGSJYHKe6ye4EjjPsWM1Ppm7MjhHRK1QYvURfbN3fkDf3Aksp3y7RnsA==" saltValue="x6s716X6wVpRxwXjkuBmrQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <mergeCells count="48">
+    <mergeCell ref="G58:K83"/>
     <mergeCell ref="E11:Q11"/>
     <mergeCell ref="E35:Q35"/>
     <mergeCell ref="E41:Q41"/>
-    <mergeCell ref="E43:Q43"/>
+    <mergeCell ref="E46:Q46"/>
     <mergeCell ref="F12:Q12"/>
     <mergeCell ref="F13:Q13"/>
     <mergeCell ref="F14:Q14"/>
@@ -4056,13 +4359,13 @@
     <mergeCell ref="F26:Q26"/>
     <mergeCell ref="F27:Q27"/>
     <mergeCell ref="F28:Q28"/>
-    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F53:G53"/>
     <mergeCell ref="E29:Q29"/>
     <mergeCell ref="E32:Q32"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="C7:F7"/>
-    <mergeCell ref="F44:Q44"/>
+    <mergeCell ref="F47:Q47"/>
     <mergeCell ref="F30:Q30"/>
     <mergeCell ref="F31:Q31"/>
     <mergeCell ref="F33:Q33"/>
@@ -4071,10 +4374,11 @@
     <mergeCell ref="F38:Q38"/>
     <mergeCell ref="F39:Q39"/>
     <mergeCell ref="F40:Q40"/>
+    <mergeCell ref="F42:Q42"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="K2:O3"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F42:Q42"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F45:Q45"/>
     <mergeCell ref="F36:Q36"/>
     <mergeCell ref="E25:Q25"/>
     <mergeCell ref="E21:Q21"/>
@@ -4085,6 +4389,8 @@
     <mergeCell ref="G5:O5"/>
     <mergeCell ref="G6:O6"/>
     <mergeCell ref="G7:O7"/>
+    <mergeCell ref="F44:Q44"/>
+    <mergeCell ref="F43:Q43"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="B12:B28">
@@ -4119,7 +4425,7 @@
       <formula>"""x"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B42">
+  <conditionalFormatting sqref="B42:B45">
     <cfRule type="notContainsBlanks" dxfId="15" priority="7">
       <formula>LEN(TRIM(B42))&gt;0</formula>
     </cfRule>
@@ -4127,9 +4433,9 @@
       <formula>"""x"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B44">
+  <conditionalFormatting sqref="B47">
     <cfRule type="notContainsBlanks" dxfId="13" priority="2">
-      <formula>LEN(TRIM(B44))&gt;0</formula>
+      <formula>LEN(TRIM(B47))&gt;0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>"""x"""</formula>
@@ -4155,14 +4461,14 @@
       <formula>LEN(TRIM(C36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
+  <conditionalFormatting sqref="C42:C45">
     <cfRule type="notContainsBlanks" dxfId="7" priority="8">
       <formula>LEN(TRIM(C42))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C44">
+  <conditionalFormatting sqref="C47">
     <cfRule type="notContainsBlanks" dxfId="6" priority="3">
-      <formula>LEN(TRIM(C44))&gt;0</formula>
+      <formula>LEN(TRIM(C47))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D28">
@@ -4185,14 +4491,14 @@
       <formula>LEN(TRIM(D36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
+  <conditionalFormatting sqref="D42:D45">
     <cfRule type="notContainsBlanks" dxfId="1" priority="6">
       <formula>LEN(TRIM(D42))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D44">
+  <conditionalFormatting sqref="D47">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(D44))&gt;0</formula>
+      <formula>LEN(TRIM(D47))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -4218,11 +4524,20 @@
     <hyperlink ref="F38" location="'8.3'!B3" display="8.3 Quando se retira a CSS, deve ser possível reconhecer a semântica dos diversos elementos" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
     <hyperlink ref="F39" location="'8.4'!B3" display="8.4 Quando se retira a CSS, a informação relevante permanece visível" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
     <hyperlink ref="F40" location="'8.5'!B3" display="8.5 A maquetização da página é feita sem recorrer ao elemento &lt;table&gt;" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="F42" location="'9.1'!B3" display="9.1 A página apresenta-se sem erros de (x)HTML" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="F44" location="'10.1'!B3" display="10.1 Nos ficheiros PDF é possível, no mínimo, extrair o conteúdo textual para formato TXT" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="F45" location="'9.1'!B3" display="9.1 A página apresenta-se sem erros de (x)HTML" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="F47" location="'10.1'!B3" display="10.1 Nos ficheiros PDF é possível, no mínimo, extrair o conteúdo textual para formato TXT" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="F44" location="'9.1'!B3" display="9.1 A página apresenta-se sem erros de (x)HTML" xr:uid="{BE67EC2F-4A76-3247-AF5C-36716425194F}"/>
+    <hyperlink ref="F43" location="'9.1'!B3" display="9.1 A página apresenta-se sem erros de (x)HTML" xr:uid="{4BAAD5B9-8BBC-D64C-B213-8C33FC4A721D}"/>
+    <hyperlink ref="F42" location="'9.1'!B3" display="9.1 A página apresenta-se sem erros de (x)HTML" xr:uid="{FA5196F9-7D94-D14B-85A2-9F2DA9054738}"/>
+    <hyperlink ref="F43:Q43" location="'9.2'!B3" display="9.2 When a modal dialog is open, the keyboard focus  (browser or assistive technologies) must be contained within the elements of the modal" xr:uid="{ECC0EAE3-1240-7F44-9108-E0970A106E18}"/>
+    <hyperlink ref="F44:Q44" location="'9.3'!B3" display="9.3 The modal dialog must have a mechanism to close it using a keyboard or any pointing device" xr:uid="{014DD4E3-86AA-1A4A-9A2B-180F4D970493}"/>
+    <hyperlink ref="F45:Q45" location="'9.4'!B3" display="9.4 When a modal dialog is closed, the focus must return to the interactive element that invoked the modal" xr:uid="{C52B2CB6-C835-B945-BC01-0D1F6467DE0D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="B43:D43" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -4246,7 +4561,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -4297,7 +4612,7 @@
     <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -4327,7 +4642,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -4365,7 +4680,7 @@
     <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -4386,7 +4701,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -4685,7 +5000,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -4736,7 +5051,7 @@
     <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -4766,7 +5081,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -4804,7 +5119,7 @@
     <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -4825,7 +5140,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -5124,14 +5439,14 @@
   <sheetData>
     <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
       <c r="D1" s="1"/>
       <c r="E1"/>
       <c r="F1" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G1"/>
       <c r="H1"/>
@@ -5175,7 +5490,7 @@
     <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -5207,7 +5522,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -5245,7 +5560,7 @@
     <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -5266,7 +5581,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -5565,14 +5880,14 @@
   <sheetData>
     <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
       <c r="D1" s="1"/>
       <c r="E1"/>
       <c r="F1" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G1"/>
       <c r="H1"/>
@@ -5616,7 +5931,7 @@
     <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -5648,7 +5963,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -5686,7 +6001,7 @@
     <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -5707,7 +6022,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -6008,14 +6323,14 @@
   <sheetData>
     <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
       <c r="D1" s="1"/>
       <c r="E1"/>
       <c r="F1" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G1"/>
       <c r="H1"/>
@@ -6059,7 +6374,7 @@
     <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -6089,7 +6404,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -6127,7 +6442,7 @@
     <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -6148,7 +6463,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -6447,14 +6762,14 @@
   <sheetData>
     <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
       <c r="D1" s="1"/>
       <c r="E1"/>
       <c r="F1" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G1"/>
       <c r="H1"/>
@@ -6498,7 +6813,7 @@
     <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -6528,7 +6843,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -6566,7 +6881,7 @@
     <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -6587,7 +6902,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6886,14 +7201,14 @@
   <sheetData>
     <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
       <c r="D1" s="1"/>
       <c r="E1"/>
       <c r="F1" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G1"/>
       <c r="H1"/>
@@ -6937,7 +7252,7 @@
     <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -6945,7 +7260,7 @@
       <c r="D3" s="6"/>
       <c r="E3"/>
       <c r="F3" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G3"/>
       <c r="H3"/>
@@ -6967,7 +7282,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -7005,7 +7320,7 @@
     <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -7026,7 +7341,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -7325,7 +7640,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -7376,7 +7691,7 @@
     <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -7406,7 +7721,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -7444,7 +7759,7 @@
     <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -7465,7 +7780,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -7764,7 +8079,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -7815,7 +8130,7 @@
     <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -7845,7 +8160,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -7883,7 +8198,7 @@
     <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -7904,7 +8219,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -8203,14 +8518,14 @@
   <sheetData>
     <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
       <c r="D1" s="1"/>
       <c r="E1"/>
       <c r="F1" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G1"/>
       <c r="H1"/>
@@ -8254,7 +8569,7 @@
     <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -8284,7 +8599,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -8322,7 +8637,7 @@
     <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -8343,7 +8658,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -8642,7 +8957,7 @@
   <sheetData>
     <row r="1" spans="1:14" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -8664,14 +8979,12 @@
     </row>
     <row r="3" spans="1:14" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>52</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="F3" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:14" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
@@ -8679,7 +8992,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="F4" s="36" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -8697,14 +9010,14 @@
     </row>
     <row r="6" spans="1:14" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -8969,22 +9282,22 @@
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B30" s="23" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B31" s="22" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B32" s="22" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="22" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.2">
@@ -8992,7 +9305,7 @@
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="21" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.2">
@@ -9000,7 +9313,7 @@
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" s="21" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -9044,14 +9357,14 @@
   <sheetData>
     <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
       <c r="D1" s="1"/>
       <c r="E1"/>
       <c r="F1" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G1"/>
       <c r="H1"/>
@@ -9095,7 +9408,7 @@
     <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -9125,7 +9438,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -9163,7 +9476,7 @@
     <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -9184,7 +9497,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -9483,14 +9796,14 @@
   <sheetData>
     <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
       <c r="D1" s="1"/>
       <c r="E1"/>
       <c r="F1" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G1"/>
       <c r="H1"/>
@@ -9534,7 +9847,7 @@
     <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -9564,7 +9877,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -9602,7 +9915,7 @@
     <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -9623,7 +9936,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -9922,14 +10235,14 @@
   <sheetData>
     <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
       <c r="D1" s="1"/>
       <c r="E1"/>
       <c r="F1" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G1"/>
       <c r="H1"/>
@@ -9973,7 +10286,7 @@
     <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -10003,7 +10316,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -10041,7 +10354,7 @@
     <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -10062,7 +10375,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -10361,14 +10674,14 @@
   <sheetData>
     <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
       <c r="D1" s="1"/>
       <c r="E1"/>
       <c r="F1" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G1"/>
       <c r="H1"/>
@@ -10412,7 +10725,7 @@
     <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -10442,7 +10755,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -10480,7 +10793,7 @@
     <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -10501,7 +10814,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -10794,20 +11107,20 @@
     <col min="2" max="4" width="3.6640625" style="5" customWidth="1"/>
     <col min="5" max="5" width="3" style="4" customWidth="1"/>
     <col min="6" max="13" width="10.83203125" style="4"/>
-    <col min="14" max="14" width="5.6640625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="19.1640625" style="4" customWidth="1"/>
     <col min="15" max="18" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
       <c r="D1" s="1"/>
       <c r="E1"/>
       <c r="F1" s="7" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="G1"/>
       <c r="H1"/>
@@ -10851,15 +11164,13 @@
     <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>5</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3"/>
       <c r="F3" s="8" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="G3"/>
       <c r="H3"/>
@@ -10881,7 +11192,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -10919,7 +11230,7 @@
     <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -10940,7 +11251,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -11223,6 +11534,1327 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{389FB273-4189-8B4E-9D22-AB15BC070584}">
+  <dimension ref="A1:R34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" style="4" customWidth="1"/>
+    <col min="2" max="4" width="3.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="3" style="4" customWidth="1"/>
+    <col min="6" max="13" width="10.6640625" style="4"/>
+    <col min="14" max="14" width="5.6640625" style="4" customWidth="1"/>
+    <col min="15" max="18" width="10.6640625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="1"/>
+      <c r="E1"/>
+      <c r="F1" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1"/>
+      <c r="L1"/>
+      <c r="M1"/>
+      <c r="N1"/>
+      <c r="O1"/>
+      <c r="P1"/>
+      <c r="Q1"/>
+      <c r="R1"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2"/>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+    </row>
+    <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3"/>
+      <c r="B3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3"/>
+      <c r="F3" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+    </row>
+    <row r="4" spans="1:18" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4"/>
+      <c r="F4" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+    </row>
+    <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6"/>
+      <c r="B6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J7" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="37"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="37"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="37"/>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G34"/>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="F4:N4"/>
+    <mergeCell ref="J8:M27"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Síntese!A1" display="voltar à página inicial" xr:uid="{F0A81139-713B-4943-A013-2698BB72706A}"/>
+    <hyperlink ref="A1:C1" location="Summary!A1" display="return to the initial page " xr:uid="{12204102-3E06-6A44-9A51-62B9C954E30A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C8E157-398E-1348-8676-1212ECF1E017}">
+  <dimension ref="A1:R34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" style="4" customWidth="1"/>
+    <col min="2" max="4" width="3.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="3" style="4" customWidth="1"/>
+    <col min="6" max="12" width="10.6640625" style="4"/>
+    <col min="13" max="13" width="28" style="4" customWidth="1"/>
+    <col min="14" max="14" width="7.33203125" style="4" customWidth="1"/>
+    <col min="15" max="18" width="10.6640625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="1"/>
+      <c r="E1"/>
+      <c r="F1" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1"/>
+      <c r="L1"/>
+      <c r="M1"/>
+      <c r="N1"/>
+      <c r="O1"/>
+      <c r="P1"/>
+      <c r="Q1"/>
+      <c r="R1"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2"/>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+    </row>
+    <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3"/>
+      <c r="B3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3"/>
+      <c r="F3" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4"/>
+      <c r="F4" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+    </row>
+    <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6"/>
+      <c r="B6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J7" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="37"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="37"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="37"/>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G34"/>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="F4:N4"/>
+    <mergeCell ref="J8:M27"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Síntese!A1" display="voltar à página inicial" xr:uid="{B76D7228-ED4A-C947-8070-638518C7DB1B}"/>
+    <hyperlink ref="A1:C1" location="Summary!A1" display="return to the initial page " xr:uid="{5631C472-701A-8549-B21D-381C7A078193}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393BFF27-D169-4A46-97A0-241BCE04976F}">
+  <dimension ref="A1:R34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" style="4" customWidth="1"/>
+    <col min="2" max="4" width="3.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="3" style="4" customWidth="1"/>
+    <col min="6" max="13" width="10.6640625" style="4"/>
+    <col min="14" max="14" width="5.6640625" style="4" customWidth="1"/>
+    <col min="15" max="18" width="10.6640625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="1"/>
+      <c r="E1"/>
+      <c r="F1" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1"/>
+      <c r="L1"/>
+      <c r="M1"/>
+      <c r="N1"/>
+      <c r="O1"/>
+      <c r="P1"/>
+      <c r="Q1"/>
+      <c r="R1"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2"/>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+    </row>
+    <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3"/>
+      <c r="B3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3"/>
+      <c r="F3" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+    </row>
+    <row r="4" spans="1:18" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4"/>
+      <c r="F4" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+    </row>
+    <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6"/>
+      <c r="B6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J7" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="37"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="37"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="37"/>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G34"/>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="F4:N4"/>
+    <mergeCell ref="J8:M27"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Síntese!A1" display="voltar à página inicial" xr:uid="{77B058AF-01D9-6F42-998A-0302FA2C18D2}"/>
+    <hyperlink ref="A1:C1" location="Summary!A1" display="return to the initial page " xr:uid="{F521E175-69A9-7742-8172-04D7BB2F32D6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:R34"/>
   <sheetViews>
@@ -11242,14 +12874,14 @@
   <sheetData>
     <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
       <c r="D1" s="1"/>
       <c r="E1"/>
       <c r="F1" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G1"/>
       <c r="H1"/>
@@ -11293,7 +12925,7 @@
     <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -11301,7 +12933,7 @@
       <c r="D3" s="6"/>
       <c r="E3"/>
       <c r="F3" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G3"/>
       <c r="H3"/>
@@ -11323,7 +12955,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -11361,7 +12993,7 @@
     <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -11382,7 +13014,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -11691,7 +13323,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -11736,7 +13368,7 @@
     <row r="3" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -11746,7 +13378,7 @@
       </c>
       <c r="E3"/>
       <c r="F3" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G3"/>
       <c r="H3"/>
@@ -11765,7 +13397,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -11797,7 +13429,7 @@
     <row r="6" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -11815,7 +13447,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -12116,7 +13748,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -12163,7 +13795,7 @@
     <row r="3" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -12193,7 +13825,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -12227,7 +13859,7 @@
     <row r="6" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -12246,7 +13878,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -12545,7 +14177,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -12594,7 +14226,7 @@
     <row r="3" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -12602,7 +14234,7 @@
       <c r="D3" s="6"/>
       <c r="E3"/>
       <c r="F3" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G3"/>
       <c r="H3"/>
@@ -12623,7 +14255,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -12659,7 +14291,7 @@
     <row r="6" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -12679,7 +14311,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -12978,7 +14610,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -13029,7 +14661,7 @@
     <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -13059,7 +14691,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -13097,7 +14729,7 @@
     <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -13118,7 +14750,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -13417,14 +15049,14 @@
   <sheetData>
     <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
       <c r="D1" s="1"/>
       <c r="E1"/>
       <c r="F1" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G1"/>
       <c r="H1"/>
@@ -13468,7 +15100,7 @@
     <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -13500,7 +15132,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -13538,7 +15170,7 @@
     <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -13559,7 +15191,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -13858,14 +15490,14 @@
   <sheetData>
     <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
       <c r="D1" s="1"/>
       <c r="E1"/>
       <c r="F1" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G1"/>
       <c r="H1"/>
@@ -13909,7 +15541,7 @@
     <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -13919,7 +15551,7 @@
       </c>
       <c r="E3"/>
       <c r="F3" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G3"/>
       <c r="H3"/>
@@ -13941,7 +15573,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -13979,7 +15611,7 @@
     <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -14000,7 +15632,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -14299,7 +15931,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -14350,7 +15982,7 @@
     <row r="3" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -14382,7 +16014,7 @@
       <c r="D4" s="1"/>
       <c r="E4"/>
       <c r="F4" s="36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
@@ -14420,7 +16052,7 @@
     <row r="6" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -14441,7 +16073,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>